<commit_message>
Added Fake Trees, Size of home (sq ft)
</commit_message>
<xml_diff>
--- a/NationalTreeSales.xlsx
+++ b/NationalTreeSales.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Files\Programming\git\team2-warm-up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmav\Documents\team2-warm-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{937C2191-4FF7-43F9-B6DC-BB30110B85F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B2D11F-C7E1-492A-9A03-3F17C728A9D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="825" windowWidth="25140" windowHeight="14055"/>
+    <workbookView xWindow="340" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NationalTreeSales" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Year</t>
-  </si>
-  <si>
-    <t>Num of Trees in millions</t>
   </si>
   <si>
     <t>Searches for "christmas trees"</t>
@@ -45,11 +52,20 @@
   <si>
     <t>Unemployment Rate, December (U-3)</t>
   </si>
+  <si>
+    <t>Num of Real Trees in millions</t>
+  </si>
+  <si>
+    <t>Num of Fake trees in millions</t>
+  </si>
+  <si>
+    <t>Avg size of home (sq ft)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -883,50 +899,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="45.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="34.7265625" customWidth="1"/>
+    <col min="3" max="3" width="39.54296875" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="5" max="5" width="45.54296875" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" customWidth="1"/>
+    <col min="7" max="7" width="35.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -952,8 +974,14 @@
       <c r="H2">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2005</v>
       </c>
@@ -979,8 +1007,14 @@
       <c r="H3">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J3">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -1006,8 +1040,14 @@
       <c r="H4">
         <v>28.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J4">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -1033,8 +1073,14 @@
       <c r="H5">
         <v>31.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J5">
+        <v>2521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -1060,8 +1106,14 @@
       <c r="H6">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>11.7</v>
+      </c>
+      <c r="J6">
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -1087,8 +1139,14 @@
       <c r="H7">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>11.7</v>
+      </c>
+      <c r="J7">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -1114,8 +1172,14 @@
       <c r="H8">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J8">
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -1141,8 +1205,14 @@
       <c r="H9">
         <v>30.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>9.5</v>
+      </c>
+      <c r="J9">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1168,8 +1238,14 @@
       <c r="H10">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>10.9</v>
+      </c>
+      <c r="J10">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -1195,8 +1271,14 @@
       <c r="H11">
         <v>33.020000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>14.7</v>
+      </c>
+      <c r="J11">
+        <v>2598</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -1222,8 +1304,14 @@
       <c r="H12">
         <v>26.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>13.9</v>
+      </c>
+      <c r="J12">
+        <v>2657</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -1249,8 +1337,14 @@
       <c r="H13">
         <v>25.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>12.5</v>
+      </c>
+      <c r="J13">
+        <v>2687</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -1276,8 +1370,14 @@
       <c r="H14">
         <v>27.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J14">
+        <v>2640</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2017</v>
       </c>
@@ -1303,8 +1403,14 @@
       <c r="H15">
         <v>27.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>21.1</v>
+      </c>
+      <c r="J15">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1330,8 +1436,14 @@
       <c r="H16">
         <v>32.799999999999997</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>23.6</v>
+      </c>
+      <c r="J16">
+        <v>2623</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1356,6 +1468,12 @@
       </c>
       <c r="H17">
         <v>32.4</v>
+      </c>
+      <c r="I17">
+        <v>24.4</v>
+      </c>
+      <c r="J17">
+        <v>2322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed xlsx to be proper order
</commit_message>
<xml_diff>
--- a/NationalTreeSales.xlsx
+++ b/NationalTreeSales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmav\Documents\team2-warm-up\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Files\Programming\git\team2-warm-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B2D11F-C7E1-492A-9A03-3F17C728A9D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30770497-0E84-4E8D-A581-EAA5E573D4D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22755" yWindow="1575" windowWidth="18960" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NationalTreeSales" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -903,20 +901,22 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.7265625" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" customWidth="1"/>
-    <col min="5" max="5" width="45.54296875" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" customWidth="1"/>
-    <col min="7" max="7" width="35.7265625" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="45.5703125" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" customWidth="1"/>
+    <col min="9" max="9" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -939,16 +939,16 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2004</v>
       </c>
@@ -972,16 +972,16 @@
         <v>5.4</v>
       </c>
       <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>2349</v>
+      </c>
+      <c r="J2">
         <v>27</v>
       </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>2349</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2005</v>
       </c>
@@ -1005,16 +1005,16 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I3">
+        <v>2434</v>
+      </c>
+      <c r="J3">
         <v>33</v>
       </c>
-      <c r="I3">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J3">
-        <v>2434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2006</v>
       </c>
@@ -1038,16 +1038,16 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I4">
+        <v>2469</v>
+      </c>
+      <c r="J4">
         <v>28.6</v>
       </c>
-      <c r="I4">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J4">
-        <v>2469</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2007</v>
       </c>
@@ -1071,16 +1071,16 @@
         <v>5</v>
       </c>
       <c r="H5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I5">
+        <v>2521</v>
+      </c>
+      <c r="J5">
         <v>31.3</v>
       </c>
-      <c r="I5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="J5">
-        <v>2521</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2008</v>
       </c>
@@ -1104,16 +1104,16 @@
         <v>7.3</v>
       </c>
       <c r="H6">
+        <v>11.7</v>
+      </c>
+      <c r="I6">
+        <v>2519</v>
+      </c>
+      <c r="J6">
         <v>28.2</v>
       </c>
-      <c r="I6">
-        <v>11.7</v>
-      </c>
-      <c r="J6">
-        <v>2519</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2009</v>
       </c>
@@ -1137,16 +1137,16 @@
         <v>9.9</v>
       </c>
       <c r="H7">
+        <v>11.7</v>
+      </c>
+      <c r="I7">
+        <v>2438</v>
+      </c>
+      <c r="J7">
         <v>28.2</v>
       </c>
-      <c r="I7">
-        <v>11.7</v>
-      </c>
-      <c r="J7">
-        <v>2438</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -1170,16 +1170,16 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I8">
+        <v>2392</v>
+      </c>
+      <c r="J8">
         <v>27</v>
       </c>
-      <c r="I8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="J8">
-        <v>2392</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2011</v>
       </c>
@@ -1203,16 +1203,16 @@
         <v>8.5</v>
       </c>
       <c r="H9">
+        <v>9.5</v>
+      </c>
+      <c r="I9">
+        <v>2480</v>
+      </c>
+      <c r="J9">
         <v>30.8</v>
       </c>
-      <c r="I9">
-        <v>9.5</v>
-      </c>
-      <c r="J9">
-        <v>2480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1236,16 +1236,16 @@
         <v>7.9</v>
       </c>
       <c r="H10">
+        <v>10.9</v>
+      </c>
+      <c r="I10">
+        <v>2505</v>
+      </c>
+      <c r="J10">
         <v>24.5</v>
       </c>
-      <c r="I10">
-        <v>10.9</v>
-      </c>
-      <c r="J10">
-        <v>2505</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2013</v>
       </c>
@@ -1269,16 +1269,16 @@
         <v>6.7</v>
       </c>
       <c r="H11">
+        <v>14.7</v>
+      </c>
+      <c r="I11">
+        <v>2598</v>
+      </c>
+      <c r="J11">
         <v>33.020000000000003</v>
       </c>
-      <c r="I11">
-        <v>14.7</v>
-      </c>
-      <c r="J11">
-        <v>2598</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -1302,16 +1302,16 @@
         <v>5.6</v>
       </c>
       <c r="H12">
+        <v>13.9</v>
+      </c>
+      <c r="I12">
+        <v>2657</v>
+      </c>
+      <c r="J12">
         <v>26.3</v>
       </c>
-      <c r="I12">
-        <v>13.9</v>
-      </c>
-      <c r="J12">
-        <v>2657</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2015</v>
       </c>
@@ -1335,16 +1335,16 @@
         <v>5</v>
       </c>
       <c r="H13">
+        <v>12.5</v>
+      </c>
+      <c r="I13">
+        <v>2687</v>
+      </c>
+      <c r="J13">
         <v>25.9</v>
       </c>
-      <c r="I13">
-        <v>12.5</v>
-      </c>
-      <c r="J13">
-        <v>2687</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2016</v>
       </c>
@@ -1368,16 +1368,16 @@
         <v>4.7</v>
       </c>
       <c r="H14">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I14">
+        <v>2640</v>
+      </c>
+      <c r="J14">
         <v>27.4</v>
       </c>
-      <c r="I14">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="J14">
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2017</v>
       </c>
@@ -1401,16 +1401,16 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="H15">
+        <v>21.1</v>
+      </c>
+      <c r="I15">
+        <v>2631</v>
+      </c>
+      <c r="J15">
         <v>27.4</v>
       </c>
-      <c r="I15">
-        <v>21.1</v>
-      </c>
-      <c r="J15">
-        <v>2631</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2018</v>
       </c>
@@ -1434,16 +1434,16 @@
         <v>3.9</v>
       </c>
       <c r="H16">
+        <v>23.6</v>
+      </c>
+      <c r="I16">
+        <v>2623</v>
+      </c>
+      <c r="J16">
         <v>32.799999999999997</v>
       </c>
-      <c r="I16">
-        <v>23.6</v>
-      </c>
-      <c r="J16">
-        <v>2623</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2019</v>
       </c>
@@ -1467,13 +1467,13 @@
         <v>3.5</v>
       </c>
       <c r="H17">
+        <v>24.4</v>
+      </c>
+      <c r="I17">
+        <v>2322</v>
+      </c>
+      <c r="J17">
         <v>32.4</v>
-      </c>
-      <c r="I17">
-        <v>24.4</v>
-      </c>
-      <c r="J17">
-        <v>2322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added found predictions, used 0s as placeholders
</commit_message>
<xml_diff>
--- a/NationalTreeSales.xlsx
+++ b/NationalTreeSales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmav\Documents\team2-warm-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B2D11F-C7E1-492A-9A03-3F17C728A9D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6454D8A-4BD5-4B4D-BD44-068CDAF3708D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NationalTreeSales" sheetId="1" r:id="rId1"/>
@@ -900,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -992,7 +992,7 @@
         <v>75</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D17" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D18" si="0">B3/C3</f>
         <v>1</v>
       </c>
       <c r="E3">
@@ -1474,6 +1474,38 @@
       </c>
       <c r="J17">
         <v>2322</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2027</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>28653</v>
+      </c>
+      <c r="F18">
+        <v>130232</v>
+      </c>
+      <c r="G18">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H18">
+        <v>28.3</v>
+      </c>
+      <c r="I18">
+        <v>30</v>
+      </c>
+      <c r="J18">
+        <v>2600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Udate File with 2027 info
</commit_message>
<xml_diff>
--- a/NationalTreeSales.xlsx
+++ b/NationalTreeSales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmav\Documents\team2-warm-up\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6454D8A-4BD5-4B4D-BD44-068CDAF3708D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B89BD07-B265-464F-BA96-B86E87F40D2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -902,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,13 +939,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -972,13 +972,13 @@
         <v>5.4</v>
       </c>
       <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>2349</v>
+      </c>
+      <c r="J2">
         <v>27</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2">
-        <v>2349</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -992,7 +992,7 @@
         <v>75</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D18" si="0">B3/C3</f>
+        <f t="shared" ref="D3:D17" si="0">B3/C3</f>
         <v>1</v>
       </c>
       <c r="E3">
@@ -1005,13 +1005,13 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I3">
+        <v>2434</v>
+      </c>
+      <c r="J3">
         <v>33</v>
-      </c>
-      <c r="I3">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J3">
-        <v>2434</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1038,13 +1038,13 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I4">
+        <v>2469</v>
+      </c>
+      <c r="J4">
         <v>28.6</v>
-      </c>
-      <c r="I4">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="J4">
-        <v>2469</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1071,13 +1071,13 @@
         <v>5</v>
       </c>
       <c r="H5">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I5">
+        <v>2521</v>
+      </c>
+      <c r="J5">
         <v>31.3</v>
-      </c>
-      <c r="I5">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="J5">
-        <v>2521</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1104,13 +1104,13 @@
         <v>7.3</v>
       </c>
       <c r="H6">
+        <v>11.7</v>
+      </c>
+      <c r="I6">
+        <v>2519</v>
+      </c>
+      <c r="J6">
         <v>28.2</v>
-      </c>
-      <c r="I6">
-        <v>11.7</v>
-      </c>
-      <c r="J6">
-        <v>2519</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1137,13 +1137,13 @@
         <v>9.9</v>
       </c>
       <c r="H7">
+        <v>11.7</v>
+      </c>
+      <c r="I7">
+        <v>2438</v>
+      </c>
+      <c r="J7">
         <v>28.2</v>
-      </c>
-      <c r="I7">
-        <v>11.7</v>
-      </c>
-      <c r="J7">
-        <v>2438</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1170,13 +1170,13 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H8">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I8">
+        <v>2392</v>
+      </c>
+      <c r="J8">
         <v>27</v>
-      </c>
-      <c r="I8">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="J8">
-        <v>2392</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1203,13 +1203,13 @@
         <v>8.5</v>
       </c>
       <c r="H9">
+        <v>9.5</v>
+      </c>
+      <c r="I9">
+        <v>2480</v>
+      </c>
+      <c r="J9">
         <v>30.8</v>
-      </c>
-      <c r="I9">
-        <v>9.5</v>
-      </c>
-      <c r="J9">
-        <v>2480</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -1236,13 +1236,13 @@
         <v>7.9</v>
       </c>
       <c r="H10">
+        <v>10.9</v>
+      </c>
+      <c r="I10">
+        <v>2505</v>
+      </c>
+      <c r="J10">
         <v>24.5</v>
-      </c>
-      <c r="I10">
-        <v>10.9</v>
-      </c>
-      <c r="J10">
-        <v>2505</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -1269,13 +1269,13 @@
         <v>6.7</v>
       </c>
       <c r="H11">
+        <v>14.7</v>
+      </c>
+      <c r="I11">
+        <v>2598</v>
+      </c>
+      <c r="J11">
         <v>33.020000000000003</v>
-      </c>
-      <c r="I11">
-        <v>14.7</v>
-      </c>
-      <c r="J11">
-        <v>2598</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1302,13 +1302,13 @@
         <v>5.6</v>
       </c>
       <c r="H12">
+        <v>13.9</v>
+      </c>
+      <c r="I12">
+        <v>2657</v>
+      </c>
+      <c r="J12">
         <v>26.3</v>
-      </c>
-      <c r="I12">
-        <v>13.9</v>
-      </c>
-      <c r="J12">
-        <v>2657</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1335,13 +1335,13 @@
         <v>5</v>
       </c>
       <c r="H13">
+        <v>12.5</v>
+      </c>
+      <c r="I13">
+        <v>2687</v>
+      </c>
+      <c r="J13">
         <v>25.9</v>
-      </c>
-      <c r="I13">
-        <v>12.5</v>
-      </c>
-      <c r="J13">
-        <v>2687</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -1368,13 +1368,13 @@
         <v>4.7</v>
       </c>
       <c r="H14">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="I14">
+        <v>2640</v>
+      </c>
+      <c r="J14">
         <v>27.4</v>
-      </c>
-      <c r="I14">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="J14">
-        <v>2640</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -1401,13 +1401,13 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="H15">
+        <v>21.1</v>
+      </c>
+      <c r="I15">
+        <v>2631</v>
+      </c>
+      <c r="J15">
         <v>27.4</v>
-      </c>
-      <c r="I15">
-        <v>21.1</v>
-      </c>
-      <c r="J15">
-        <v>2631</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1434,13 +1434,13 @@
         <v>3.9</v>
       </c>
       <c r="H16">
+        <v>23.6</v>
+      </c>
+      <c r="I16">
+        <v>2623</v>
+      </c>
+      <c r="J16">
         <v>32.799999999999997</v>
-      </c>
-      <c r="I16">
-        <v>23.6</v>
-      </c>
-      <c r="J16">
-        <v>2623</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
@@ -1467,13 +1467,13 @@
         <v>3.5</v>
       </c>
       <c r="H17">
+        <v>24.4</v>
+      </c>
+      <c r="I17">
+        <v>2322</v>
+      </c>
+      <c r="J17">
         <v>32.4</v>
-      </c>
-      <c r="I17">
-        <v>24.4</v>
-      </c>
-      <c r="J17">
-        <v>2322</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
@@ -1499,13 +1499,13 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="H18">
+        <v>30</v>
+      </c>
+      <c r="I18">
+        <v>2600</v>
+      </c>
+      <c r="J18">
         <v>28.3</v>
-      </c>
-      <c r="I18">
-        <v>30</v>
-      </c>
-      <c r="J18">
-        <v>2600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>